<commit_message>
Added More to Mapping
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -11,12 +11,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="123">
   <si>
     <t>port_waste</t>
   </si>
   <si>
-    <t>master</t>
+    <t>mastersheet</t>
+  </si>
+  <si>
+    <t>Reference #</t>
   </si>
   <si>
     <t>Site Description</t>
@@ -31,6 +34,25 @@
     <t>Type</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1206912</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916110) - 2.5</t>
+    </r>
+  </si>
+  <si>
     <t>T-4</t>
   </si>
   <si>
@@ -41,6 +63,25 @@
   </si>
   <si>
     <t>Garbage</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1428233</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916110)-2.8</t>
+    </r>
   </si>
   <si>
     <t>Waste, Special,
@@ -50,16 +91,1184 @@
     <t>MID</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">1328588 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>- 2.23</t>
+    </r>
+  </si>
+  <si>
     <t>Guard House</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1208123</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916226) 2.17</t>
+    </r>
+  </si>
+  <si>
     <t>Varies</t>
   </si>
   <si>
     <t>Commingle</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1206912</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916110)- 2.7</t>
+    </r>
+  </si>
+  <si>
+    <t>Organics</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1206912</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916110) - 2.21</t>
+    </r>
+  </si>
+  <si>
+    <t>Glass</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">1328588 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>- 2.22</t>
+    </r>
+  </si>
+  <si>
     <t>Comingle</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207131</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916129.1)-2.10</t>
+    </r>
+  </si>
+  <si>
+    <t>MFM</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207131</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916129.1 )- 2.9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207240</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>- 2.15</t>
+    </r>
+  </si>
+  <si>
+    <t>T-6</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207240</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - 2.14</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207349</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - 2.41</t>
+    </r>
+  </si>
+  <si>
+    <t>Waste, Special,
+Sweeper</t>
+  </si>
+  <si>
+    <t>Street Sweep Debris</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>2191511</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - 2.43</t>
+    </r>
+  </si>
+  <si>
+    <t>T-6 Security Shack</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">1209335 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>- 2.42</t>
+    </r>
+  </si>
+  <si>
+    <t>Misc.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207240</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - 2.12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207240</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - 2.16</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207240</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - 2.18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>2191511</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - 2.44</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207458</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916145) - 3.1</t>
+    </r>
+  </si>
+  <si>
+    <t>Dredge</t>
+  </si>
+  <si>
+    <t>NAV</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207458</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916145) - 3.3</t>
+    </r>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207458</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916145) - 3.31</t>
+    </r>
+  </si>
+  <si>
+    <t>Trash- On  Barge</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207458</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916145) - 3.32</t>
+    </r>
+  </si>
+  <si>
+    <t>Trash-Barge exchange box</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <strike val="1"/>
+        <sz val="6"/>
+        <color indexed="19"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207458</t>
+    </r>
+    <r>
+      <rPr>
+        <strike val="1"/>
+        <sz val="6"/>
+        <color indexed="19"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916145) - 3.2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207458</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916145) - 3.21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207458</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916145)</t>
+    </r>
+  </si>
+  <si>
+    <t>Special Projects</t>
+  </si>
+  <si>
+    <t>Misc./Other</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1205692</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916013) - 4.2</t>
+    </r>
+  </si>
+  <si>
+    <t>T-1</t>
+  </si>
+  <si>
+    <t>TERM</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1205692</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916013) - 4.5</t>
+    </r>
+  </si>
+  <si>
+    <t>T-2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207905-(4.39)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>2358160 CONCESSIONS LN11</t>
+    </r>
+  </si>
+  <si>
+    <t>Special Events</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1205692</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916013) - 4.6</t>
+    </r>
+  </si>
+  <si>
+    <t>T-3</t>
+  </si>
+  <si>
+    <t>South Commingle</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1205692</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916013) - 4.4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <strike val="1"/>
+        <sz val="6"/>
+        <color indexed="19"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1205692</t>
+    </r>
+    <r>
+      <rPr>
+        <strike val="1"/>
+        <sz val="6"/>
+        <color indexed="19"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916013) - 4.3</t>
+    </r>
+  </si>
+  <si>
+    <t>T-5</t>
+  </si>
+  <si>
+    <t>Plastic</t>
+  </si>
+  <si>
+    <t>Plastics (i.e, film, rigids)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1205692</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916013) - 4.1</t>
+    </r>
+  </si>
+  <si>
+    <t>T-7</t>
+  </si>
+  <si>
+    <t>North Commingle</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207896</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916196)- 4.40</t>
+    </r>
+  </si>
+  <si>
+    <t>Terminal</t>
+  </si>
+  <si>
+    <t>Organics (Food Waste)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1207905</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>-4.39</t>
+    </r>
+  </si>
+  <si>
+    <t>Recycling Varies</t>
+  </si>
+  <si>
+    <t>CHECK CELL NOTES</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1208888</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916293) - 4.55</t>
+    </r>
+  </si>
+  <si>
+    <t>PQ1</t>
+  </si>
+  <si>
+    <t>PACR</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <strike val="1"/>
+        <sz val="6"/>
+        <color indexed="19"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1208888</t>
+    </r>
+    <r>
+      <rPr>
+        <strike val="1"/>
+        <sz val="6"/>
+        <color indexed="19"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916293) - 4.56</t>
+    </r>
+  </si>
+  <si>
+    <t>Headquarters</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1208888</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916293) - 4.52</t>
+    </r>
+  </si>
+  <si>
+    <t>PQ2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1208888</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916293) - 4.53</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1208888</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916293) - 4.54</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1209007</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916315) - 4.58</t>
+    </r>
+  </si>
+  <si>
+    <t>Deicing Facility</t>
+  </si>
+  <si>
+    <t>DEICING</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1209007</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916315) - 4.59</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1206029</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916056) - 4.17</t>
+    </r>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>FIRE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1206029</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916056) - 4.16</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1206029</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916056) - 4.15</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1206029</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916056) - 4.49</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1206247</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916064.1) -4.18</t>
+    </r>
+  </si>
+  <si>
+    <t>Maint. Bldgs.,
+Annex</t>
+  </si>
+  <si>
+    <t>MX</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1206138</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916064) - 4.19</t>
+    </r>
+  </si>
+  <si>
+    <t>M-9 Maint. Bldgs.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1206138</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916064) - 4.25</t>
+    </r>
+  </si>
+  <si>
+    <t>Maint. Bldgs.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1206138</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916064) - 4.20</t>
+    </r>
+  </si>
+  <si>
+    <t>Waste, Special,
+Left, Sweeper</t>
+  </si>
+  <si>
+    <t>Sweeper</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1206138</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916064) - 4.23</t>
+    </r>
+  </si>
+  <si>
+    <t>Waste, Special,
+Right Drain,
+Basin</t>
+  </si>
+  <si>
+    <t>Storm Drain</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <strike val="1"/>
+        <sz val="6"/>
+        <color indexed="19"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1205701</t>
+    </r>
+    <r>
+      <rPr>
+        <strike val="1"/>
+        <sz val="6"/>
+        <color indexed="19"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916021) - 4.8</t>
+    </r>
+  </si>
+  <si>
+    <t>CUP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1206684</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916080) - 4.38</t>
+    </r>
+  </si>
+  <si>
+    <t>GT Hold Lot</t>
+  </si>
+  <si>
+    <t>PARKING</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1206684</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916080) - 4.39</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <strike val="1"/>
+        <sz val="6"/>
+        <color indexed="19"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1205810</t>
+    </r>
+    <r>
+      <rPr>
+        <strike val="1"/>
+        <sz val="6"/>
+        <color indexed="19"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(916048) - 4.9</t>
+    </r>
+  </si>
+  <si>
+    <t>CRCI</t>
+  </si>
+  <si>
+    <t>CONSTRUCTION OFF</t>
   </si>
 </sst>
 </file>
@@ -69,7 +1278,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -81,12 +1290,53 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="6"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <strike val="1"/>
+      <sz val="6"/>
+      <color indexed="19"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <strike val="1"/>
+      <sz val="6"/>
+      <color indexed="19"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,13 +1345,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="11"/>
+        <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -113,30 +1357,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="14"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="15"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="16"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -145,79 +1371,332 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="10"/>
+      <left style="medium">
+        <color indexed="8"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
+      <right style="medium">
+        <color indexed="11"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
+      <left style="medium">
+        <color indexed="11"/>
+      </left>
+      <right style="medium">
+        <color indexed="11"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
+      <left style="medium">
+        <color indexed="11"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
       </right>
-      <top style="thin">
-        <color indexed="10"/>
+      <top style="medium">
+        <color indexed="8"/>
       </top>
-      <bottom style="thin">
-        <color indexed="10"/>
+      <bottom style="medium">
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="18"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
       </bottom>
       <diagonal/>
     </border>
@@ -227,60 +1706,153 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -299,14 +1871,17 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="fffbbc04"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff34a853"/>
+      <rgbColor rgb="fff7f2de"/>
+      <rgbColor rgb="ff6b4e1b"/>
+      <rgbColor rgb="ff929292"/>
+      <rgbColor rgb="fffdad00"/>
+      <rgbColor rgb="ff7f7f7f"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="fff7cb4d"/>
-      <rgbColor rgb="ff8bc34a"/>
-      <rgbColor rgb="fffef8e3"/>
-      <rgbColor rgb="ffeef7e3"/>
+      <rgbColor rgb="ff89847f"/>
+      <rgbColor rgb="ffc8c8c8"/>
+      <rgbColor rgb="ffbfbfbf"/>
+      <rgbColor rgb="ffe3e3e3"/>
+      <rgbColor rgb="ffdd0806"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1341,11 +2916,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="12.6719" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.3516" style="1" customWidth="1"/>
@@ -1358,124 +2933,987 @@
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
-      <c r="C1" t="s" s="4">
+      <c r="C1" s="4"/>
+      <c r="D1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="7">
+      <c r="A2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="8">
+      <c r="B2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="C2" t="s" s="9">
+      <c r="C2" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="D2" t="s" s="9">
+      <c r="D2" t="s" s="7">
         <v>5</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" t="s" s="8">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="10">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s" s="11">
+      <c r="A3" t="s" s="9">
         <v>7</v>
       </c>
+      <c r="B3" t="s" s="10">
+        <v>8</v>
+      </c>
       <c r="C3" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s" s="13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" ht="24.65" customHeight="1">
+      <c r="A4" t="s" s="14">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s" s="15">
         <v>8</v>
       </c>
-      <c r="D3" t="s" s="11">
+      <c r="C4" t="s" s="16">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s" s="17">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" t="s" s="19">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s" s="20">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s" s="21">
         <v>9</v>
       </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" ht="24.65" customHeight="1">
-      <c r="A4" t="s" s="12">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s" s="13">
+      <c r="D5" t="s" s="22">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="14">
+      <c r="E5" t="s" s="23">
         <v>11</v>
       </c>
-      <c r="D4" t="s" s="14">
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" t="s" s="14">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s" s="15">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s" s="16">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s" s="17">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s" s="18">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" t="s" s="19">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s" s="20">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s" s="21">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s" s="22">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s" s="23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" t="s" s="14">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s" s="15">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s" s="17">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s" s="18">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" t="s" s="19">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s" s="20">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s" s="21">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s" s="22">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s" s="23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" t="s" s="14">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s" s="15">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s" s="16">
         <v>9</v>
       </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="10">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s" s="11">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s" s="11">
+      <c r="D10" t="s" s="17">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" ht="13.65" customHeight="1">
+      <c r="A11" t="s" s="19">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s" s="20">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s" s="21">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s" s="22">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s" s="23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" ht="13.65" customHeight="1">
+      <c r="A12" t="s" s="14">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s" s="15">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s" s="17">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" ht="13.65" customHeight="1">
+      <c r="A13" t="s" s="19">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s" s="20">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s" s="21">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s" s="22">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s" s="23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" ht="13.65" customHeight="1">
+      <c r="A14" t="s" s="14">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s" s="15">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s" s="24">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s" s="17">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s" s="18">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" ht="13.65" customHeight="1">
+      <c r="A15" t="s" s="19">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s" s="25">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s" s="21">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s" s="22">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s" s="23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" ht="13.65" customHeight="1">
+      <c r="A16" t="s" s="14">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s" s="15">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s" s="16">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s" s="17">
+        <v>31</v>
+      </c>
+      <c r="E16" t="s" s="18">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" ht="13.65" customHeight="1">
+      <c r="A17" t="s" s="19">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s" s="20">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s" s="21">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s" s="22">
+        <v>31</v>
+      </c>
+      <c r="E17" t="s" s="23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" ht="13.65" customHeight="1">
+      <c r="A18" t="s" s="14">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s" s="15">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s" s="16">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s" s="17">
+        <v>31</v>
+      </c>
+      <c r="E18" t="s" s="18">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" ht="13.65" customHeight="1">
+      <c r="A19" t="s" s="19">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s" s="20">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s" s="21">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s" s="22">
+        <v>31</v>
+      </c>
+      <c r="E19" t="s" s="23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" ht="13.65" customHeight="1">
+      <c r="A20" t="s" s="14">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s" s="15">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s" s="16">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s" s="17">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s" s="18">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" ht="13.65" customHeight="1">
+      <c r="A21" t="s" s="19">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s" s="20">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s" s="21">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s" s="22">
+        <v>46</v>
+      </c>
+      <c r="E21" t="s" s="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" ht="13.65" customHeight="1">
+      <c r="A22" t="s" s="14">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s" s="26">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s" s="17">
+        <v>46</v>
+      </c>
+      <c r="E22" t="s" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" ht="13.65" customHeight="1">
+      <c r="A23" t="s" s="27">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s" s="20">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s" s="28">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s" s="22">
+        <v>46</v>
+      </c>
+      <c r="E23" t="s" s="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" ht="13.65" customHeight="1">
+      <c r="A24" t="s" s="29">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s" s="15">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s" s="24">
+        <v>52</v>
+      </c>
+      <c r="D24" t="s" s="17">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" ht="13.65" customHeight="1">
+      <c r="A25" t="s" s="30">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s" s="20">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s" s="21">
+        <v>25</v>
+      </c>
+      <c r="D25" t="s" s="22">
+        <v>46</v>
+      </c>
+      <c r="E25" t="s" s="23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" ht="13.65" customHeight="1">
+      <c r="A26" t="s" s="31">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s" s="15">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s" s="16">
+        <v>25</v>
+      </c>
+      <c r="D26" t="s" s="17">
+        <v>46</v>
+      </c>
+      <c r="E26" t="s" s="18">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" ht="13.65" customHeight="1">
+      <c r="A27" t="s" s="32">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s" s="25">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s" s="21">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s" s="22">
+        <v>46</v>
+      </c>
+      <c r="E27" t="s" s="23">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" ht="13.65" customHeight="1">
+      <c r="A28" t="s" s="33">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s" s="15">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s" s="17">
+        <v>60</v>
+      </c>
+      <c r="E28" t="s" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" ht="13.65" customHeight="1">
+      <c r="A29" t="s" s="32">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s" s="20">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s" s="21">
+        <v>9</v>
+      </c>
+      <c r="D29" t="s" s="22">
+        <v>60</v>
+      </c>
+      <c r="E29" t="s" s="23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" ht="13.65" customHeight="1">
+      <c r="A30" t="s" s="33">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s" s="26">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s" s="16">
+        <v>18</v>
+      </c>
+      <c r="D30" t="s" s="17">
+        <v>60</v>
+      </c>
+      <c r="E30" t="s" s="18">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" ht="13.65" customHeight="1">
+      <c r="A31" t="s" s="32">
+        <v>65</v>
+      </c>
+      <c r="B31" t="s" s="20">
+        <v>66</v>
+      </c>
+      <c r="C31" t="s" s="21">
+        <v>67</v>
+      </c>
+      <c r="D31" t="s" s="22">
+        <v>60</v>
+      </c>
+      <c r="E31" t="s" s="23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" ht="13.65" customHeight="1">
+      <c r="A32" t="s" s="33">
+        <v>68</v>
+      </c>
+      <c r="B32" t="s" s="15">
         <v>8</v>
       </c>
-      <c r="D5" t="s" s="11">
+      <c r="C32" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="D32" t="s" s="17">
+        <v>60</v>
+      </c>
+      <c r="E32" t="s" s="18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" ht="13.65" customHeight="1">
+      <c r="A33" t="s" s="32">
+        <v>69</v>
+      </c>
+      <c r="B33" t="s" s="20">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s" s="21">
+        <v>71</v>
+      </c>
+      <c r="D33" t="s" s="22">
+        <v>60</v>
+      </c>
+      <c r="E33" t="s" s="23">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" ht="13.65" customHeight="1">
+      <c r="A34" t="s" s="33">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s" s="15">
+        <v>74</v>
+      </c>
+      <c r="C34" t="s" s="24">
+        <v>75</v>
+      </c>
+      <c r="D34" t="s" s="17">
+        <v>60</v>
+      </c>
+      <c r="E34" t="s" s="18">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" ht="13.65" customHeight="1">
+      <c r="A35" t="s" s="32">
+        <v>76</v>
+      </c>
+      <c r="B35" t="s" s="20">
+        <v>77</v>
+      </c>
+      <c r="C35" t="s" s="21">
+        <v>21</v>
+      </c>
+      <c r="D35" t="s" s="22">
+        <v>60</v>
+      </c>
+      <c r="E35" t="s" s="23">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" ht="13.65" customHeight="1">
+      <c r="A36" t="s" s="33">
+        <v>79</v>
+      </c>
+      <c r="B36" t="s" s="26">
+        <v>64</v>
+      </c>
+      <c r="C36" t="s" s="24">
+        <v>80</v>
+      </c>
+      <c r="D36" t="s" s="17">
+        <v>60</v>
+      </c>
+      <c r="E36" t="s" s="18">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" ht="13.65" customHeight="1">
+      <c r="A37" t="s" s="32">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s" s="25">
+        <v>83</v>
+      </c>
+      <c r="C37" t="s" s="21">
         <v>9</v>
       </c>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="12">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s" s="14">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s" s="14">
-        <v>14</v>
-      </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" t="s" s="10">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="11">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="D37" t="s" s="22">
+        <v>84</v>
+      </c>
+      <c r="E37" t="s" s="23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" ht="13.65" customHeight="1">
+      <c r="A38" t="s" s="33">
+        <v>85</v>
+      </c>
+      <c r="B38" t="s" s="34">
+        <v>86</v>
+      </c>
+      <c r="C38" t="s" s="35">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s" s="17">
+        <v>84</v>
+      </c>
+      <c r="E38" t="s" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" ht="13.65" customHeight="1">
+      <c r="A39" t="s" s="32">
+        <v>87</v>
+      </c>
+      <c r="B39" t="s" s="25">
+        <v>88</v>
+      </c>
+      <c r="C39" t="s" s="21">
+        <v>25</v>
+      </c>
+      <c r="D39" t="s" s="22">
+        <v>84</v>
+      </c>
+      <c r="E39" t="s" s="23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" ht="13.65" customHeight="1">
+      <c r="A40" t="s" s="33">
+        <v>89</v>
+      </c>
+      <c r="B40" t="s" s="26">
+        <v>86</v>
+      </c>
+      <c r="C40" t="s" s="16">
+        <v>25</v>
+      </c>
+      <c r="D40" t="s" s="17">
+        <v>84</v>
+      </c>
+      <c r="E40" t="s" s="18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" ht="13.65" customHeight="1">
+      <c r="A41" t="s" s="32">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s" s="25">
+        <v>86</v>
+      </c>
+      <c r="C41" t="s" s="21">
+        <v>21</v>
+      </c>
+      <c r="D41" t="s" s="22">
+        <v>84</v>
+      </c>
+      <c r="E41" t="s" s="36">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" ht="13.65" customHeight="1">
+      <c r="A42" t="s" s="33">
+        <v>91</v>
+      </c>
+      <c r="B42" t="s" s="26">
+        <v>92</v>
+      </c>
+      <c r="C42" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s" s="17">
+        <v>93</v>
+      </c>
+      <c r="E42" t="s" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" ht="13.65" customHeight="1">
+      <c r="A43" t="s" s="32">
+        <v>94</v>
+      </c>
+      <c r="B43" t="s" s="25">
+        <v>92</v>
+      </c>
+      <c r="C43" t="s" s="21">
+        <v>25</v>
+      </c>
+      <c r="D43" t="s" s="22">
+        <v>93</v>
+      </c>
+      <c r="E43" t="s" s="23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" ht="13.65" customHeight="1">
+      <c r="A44" t="s" s="33">
+        <v>95</v>
+      </c>
+      <c r="B44" t="s" s="26">
+        <v>96</v>
+      </c>
+      <c r="C44" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s" s="17">
+        <v>97</v>
+      </c>
+      <c r="E44" t="s" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" ht="13.65" customHeight="1">
+      <c r="A45" t="s" s="32">
+        <v>98</v>
+      </c>
+      <c r="B45" t="s" s="25">
+        <v>96</v>
+      </c>
+      <c r="C45" t="s" s="28">
+        <v>19</v>
+      </c>
+      <c r="D45" t="s" s="22">
+        <v>97</v>
+      </c>
+      <c r="E45" t="s" s="23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" ht="13.65" customHeight="1">
+      <c r="A46" t="s" s="33">
+        <v>99</v>
+      </c>
+      <c r="B46" t="s" s="26">
+        <v>96</v>
+      </c>
+      <c r="C46" t="s" s="16">
+        <v>23</v>
+      </c>
+      <c r="D46" t="s" s="17">
+        <v>97</v>
+      </c>
+      <c r="E46" t="s" s="18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" ht="13.65" customHeight="1">
+      <c r="A47" t="s" s="32">
+        <v>100</v>
+      </c>
+      <c r="B47" t="s" s="25">
+        <v>96</v>
+      </c>
+      <c r="C47" t="s" s="21">
+        <v>21</v>
+      </c>
+      <c r="D47" t="s" s="22">
+        <v>97</v>
+      </c>
+      <c r="E47" t="s" s="23">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" ht="13.65" customHeight="1">
+      <c r="A48" t="s" s="33">
+        <v>101</v>
+      </c>
+      <c r="B48" t="s" s="26">
+        <v>102</v>
+      </c>
+      <c r="C48" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s" s="17">
+        <v>103</v>
+      </c>
+      <c r="E48" t="s" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" ht="13.65" customHeight="1">
+      <c r="A49" t="s" s="32">
+        <v>104</v>
+      </c>
+      <c r="B49" t="s" s="25">
+        <v>105</v>
+      </c>
+      <c r="C49" t="s" s="21">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s" s="22">
+        <v>103</v>
+      </c>
+      <c r="E49" t="s" s="23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" ht="13.65" customHeight="1">
+      <c r="A50" t="s" s="33">
+        <v>106</v>
+      </c>
+      <c r="B50" t="s" s="26">
+        <v>107</v>
+      </c>
+      <c r="C50" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D50" t="s" s="17">
+        <v>103</v>
+      </c>
+      <c r="E50" t="s" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" ht="13.65" customHeight="1">
+      <c r="A51" t="s" s="32">
+        <v>108</v>
+      </c>
+      <c r="B51" t="s" s="25">
+        <v>107</v>
+      </c>
+      <c r="C51" t="s" s="28">
+        <v>109</v>
+      </c>
+      <c r="D51" t="s" s="22">
+        <v>103</v>
+      </c>
+      <c r="E51" t="s" s="23">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" ht="13.65" customHeight="1">
+      <c r="A52" t="s" s="33">
+        <v>111</v>
+      </c>
+      <c r="B52" t="s" s="26">
+        <v>107</v>
+      </c>
+      <c r="C52" t="s" s="24">
+        <v>112</v>
+      </c>
+      <c r="D52" t="s" s="17">
+        <v>103</v>
+      </c>
+      <c r="E52" t="s" s="18">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" ht="13.65" customHeight="1">
+      <c r="A53" t="s" s="32">
+        <v>114</v>
+      </c>
+      <c r="B53" t="s" s="37">
+        <v>115</v>
+      </c>
+      <c r="C53" t="s" s="38">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s" s="22">
+        <v>103</v>
+      </c>
+      <c r="E53" t="s" s="23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" ht="13.65" customHeight="1">
+      <c r="A54" t="s" s="33">
+        <v>116</v>
+      </c>
+      <c r="B54" t="s" s="26">
+        <v>117</v>
+      </c>
+      <c r="C54" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D54" t="s" s="17">
+        <v>118</v>
+      </c>
+      <c r="E54" t="s" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" ht="13.65" customHeight="1">
+      <c r="A55" t="s" s="32">
+        <v>119</v>
+      </c>
+      <c r="B55" t="s" s="25">
+        <v>117</v>
+      </c>
+      <c r="C55" t="s" s="21">
+        <v>9</v>
+      </c>
+      <c r="D55" t="s" s="22">
+        <v>118</v>
+      </c>
+      <c r="E55" t="s" s="23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" ht="13.65" customHeight="1">
+      <c r="A56" t="s" s="33">
+        <v>120</v>
+      </c>
+      <c r="B56" t="s" s="34">
+        <v>121</v>
+      </c>
+      <c r="C56" t="s" s="35">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s" s="17">
+        <v>122</v>
+      </c>
+      <c r="E56" t="s" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" ht="13.65" customHeight="1">
+      <c r="A57" s="39"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="43"/>
+    </row>
+    <row r="58" ht="13.65" customHeight="1">
+      <c r="A58" s="44"/>
+      <c r="B58" s="45"/>
+      <c r="C58" s="46"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="48"/>
+    </row>
+    <row r="59" ht="13.65" customHeight="1">
+      <c r="A59" s="39"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="42"/>
+      <c r="E59" s="43"/>
+    </row>
+    <row r="60" ht="13.65" customHeight="1">
+      <c r="A60" s="44"/>
+      <c r="B60" s="45"/>
+      <c r="C60" s="46"/>
+      <c r="D60" s="47"/>
+      <c r="E60" s="48"/>
+    </row>
+    <row r="61" ht="13.65" customHeight="1">
+      <c r="A61" s="39"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="42"/>
+      <c r="E61" s="43"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>